<commit_message>
I don't know, alot
</commit_message>
<xml_diff>
--- a/src/excel_db_loaders/data.xlsx
+++ b/src/excel_db_loaders/data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ω Carpe Diem\programming\portafolio\src\excel_db_loaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA24E20-BCA7-4AFC-B689-CC0C7E83672A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF25AB8-3A0A-4FE5-BBA0-0334C1DF2D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D5E59E72-371D-46EC-A17D-B18FA0163931}"/>
   </bookViews>
   <sheets>
     <sheet name="personal_info" sheetId="1" r:id="rId1"/>
+    <sheet name="programming_languages" sheetId="2" r:id="rId2"/>
+    <sheet name="other_skills" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>first_name</t>
   </si>
@@ -65,6 +67,33 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>Software engineer</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/tomislav-vesic-324569157</t>
+  </si>
+  <si>
+    <t>https://github.com/tomislavvesic</t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>14.02.1997</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Rijeka</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
   </si>
 </sst>
 </file>
@@ -109,14 +138,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,21 +462,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68D0D7D-1E2C-4DEC-A959-A6E03F32FA00}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="13.109375" style="1"/>
+    <col min="2" max="2" width="11.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="13.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,19 +493,28 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -478,13 +523,59 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E2847228-D54C-48D0-84F4-301C930412E2}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{953A6EF2-ADBE-432B-9903-FC17BBBD2C4E}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{2C7634B8-5ED2-4F64-9591-0B2973AE5B1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981EE173-0D44-4564-8556-6EB4FEC3FB87}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117CB573-1BF8-4997-BC55-BDE801C36C8A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add database read and write functionalities
</commit_message>
<xml_diff>
--- a/src/excel_db_loaders/data.xlsx
+++ b/src/excel_db_loaders/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ω Carpe Diem\programming\portafolio\src\excel_db_loaders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF25AB8-3A0A-4FE5-BBA0-0334C1DF2D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6C083C-5F6C-4C16-8937-437858C6492C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D5E59E72-371D-46EC-A17D-B18FA0163931}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D5E59E72-371D-46EC-A17D-B18FA0163931}"/>
   </bookViews>
   <sheets>
     <sheet name="personal_info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>first_name</t>
   </si>
@@ -94,6 +94,45 @@
   </si>
   <si>
     <t>state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good day everyone and welcome to my portfolio. \n  My name is Tomislav and I have been web developer for ~3 years. My focus have using Angular as a frontend and Python as a backend solution. \n In here you can find some basic info about me and projects I am usually workon on in my free time. Don't get blown away with all these awesome ideas. Feel free to contact me if you want to give me a tumbs up! </t>
+  </si>
+  <si>
+    <t>programming_language</t>
+  </si>
+  <si>
+    <t>knowledge</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Typescript</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>CSS/SCSS</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Amazon AWS</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>other_skills</t>
   </si>
 </sst>
 </file>
@@ -141,12 +180,14 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68D0D7D-1E2C-4DEC-A959-A6E03F32FA00}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +520,8 @@
     <col min="7" max="7" width="18.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="21.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="13.109375" style="1"/>
+    <col min="10" max="10" width="70.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="13.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -514,7 +556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -541,6 +583,9 @@
       </c>
       <c r="I2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -556,26 +601,125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981EE173-0D44-4564-8556-6EB4FEC3FB87}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117CB573-1BF8-4997-BC55-BDE801C36C8A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>